<commit_message>
Hooks a Senaryo sonuçlaır için Excel yazma eklendi
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
+++ b/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="8970"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="8970" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,52 +63,52 @@
     <t>bes</t>
   </si>
   <si>
-    <t>ulis1111</t>
-  </si>
-  <si>
-    <t>ulis1122</t>
-  </si>
-  <si>
-    <t>ulis1133</t>
-  </si>
-  <si>
-    <t>ulis1144</t>
-  </si>
-  <si>
-    <t>ulis1154</t>
-  </si>
-  <si>
-    <t>ulis1164</t>
-  </si>
-  <si>
-    <t>ulis1174</t>
-  </si>
-  <si>
-    <t>ulis1184</t>
-  </si>
-  <si>
-    <t>ubs13</t>
-  </si>
-  <si>
-    <t>ubs141</t>
-  </si>
-  <si>
-    <t>ubs152</t>
-  </si>
-  <si>
-    <t>ubs162</t>
-  </si>
-  <si>
-    <t>ubs172</t>
-  </si>
-  <si>
-    <t>ubs182</t>
-  </si>
-  <si>
-    <t>ubs192</t>
-  </si>
-  <si>
-    <t>ubs202</t>
+    <t>ulais1145</t>
+  </si>
+  <si>
+    <t>ulais1146</t>
+  </si>
+  <si>
+    <t>ulais1147</t>
+  </si>
+  <si>
+    <t>ulais1148</t>
+  </si>
+  <si>
+    <t>ulais1149</t>
+  </si>
+  <si>
+    <t>ulais1150</t>
+  </si>
+  <si>
+    <t>ulais1151</t>
+  </si>
+  <si>
+    <t>ulais1152</t>
+  </si>
+  <si>
+    <t>urbs13</t>
+  </si>
+  <si>
+    <t>urbs14</t>
+  </si>
+  <si>
+    <t>urbs15</t>
+  </si>
+  <si>
+    <t>urbs16</t>
+  </si>
+  <si>
+    <t>urbs17</t>
+  </si>
+  <si>
+    <t>urbs18</t>
+  </si>
+  <si>
+    <t>urbs19</t>
+  </si>
+  <si>
+    <t>urbs20</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>